<commit_message>
Deployed 2b55553 with MkDocs version: 1.6.1
</commit_message>
<xml_diff>
--- a/linearni_algerbra_diskretni_mat/Algebra_TABULKA.xlsx
+++ b/linearni_algerbra_diskretni_mat/Algebra_TABULKA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dejvi\Plocha\TUL\docs\linearni_algerbra_diskretni_mat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC58CA9-E5C8-4381-98F0-53C3235A680B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17000595-319E-46A8-947D-5B1F406AF210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="13023" tabRatio="567" xr2:uid="{0AD5C3A5-6B82-437D-9C85-E9151057B14B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="100">
   <si>
     <t>Známka</t>
   </si>
@@ -251,16 +251,91 @@
     <t>blbost</t>
   </si>
   <si>
-    <t>ještě zkusim znovu</t>
-  </si>
-  <si>
     <t>Obtížnost/Popisek</t>
   </si>
   <si>
     <t>dá se v tom chybovat</t>
   </si>
   <si>
-    <t>je to dlohý docela, hard</t>
+    <t>tohle je lehčí než zobrazení</t>
+  </si>
+  <si>
+    <t>praktické téma, docela jde</t>
+  </si>
+  <si>
+    <t>podobné 1 ale je tam par věci  co nejsou zastak jednoduchy</t>
+  </si>
+  <si>
+    <t>proste tohle nam říká zda mame vůbec reseni</t>
+  </si>
+  <si>
+    <t>je to nic moc ale není to až tak dlouhy</t>
+  </si>
+  <si>
+    <t>docela jde, něco vim prakticky</t>
+  </si>
+  <si>
+    <t>podobné 11 ale mozna trosku lehci</t>
+  </si>
+  <si>
+    <t>jednoduší než téma 7</t>
+  </si>
+  <si>
+    <t>není to ažtak obtížné</t>
+  </si>
+  <si>
+    <t>tohle jde</t>
+  </si>
+  <si>
+    <t>15 tema bylo lepsi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">narocnejsi kvuli množství textu </t>
+  </si>
+  <si>
+    <t>asi nejlehčí téma</t>
+  </si>
+  <si>
+    <t>docela kratky, jde to</t>
+  </si>
+  <si>
+    <t>ty priklady hodne pomahaji</t>
+  </si>
+  <si>
+    <t>trochu se to podobá 1</t>
+  </si>
+  <si>
+    <t>nedelat chyby v GEM</t>
+  </si>
+  <si>
+    <t>vzorců tam je extrémně moc</t>
+  </si>
+  <si>
+    <t>extrém</t>
+  </si>
+  <si>
+    <t>prakticky trochu podobné tématu 11 a navazuje to na tema 22</t>
+  </si>
+  <si>
+    <t>jde to</t>
+  </si>
+  <si>
+    <t>druhy nejlehci</t>
+  </si>
+  <si>
+    <t>neumim to rict presne podle tech vet nektery věci</t>
+  </si>
+  <si>
+    <t>hodne v poho</t>
+  </si>
+  <si>
+    <t>jde to, jsou tam věci co se daji snadno zapomenout</t>
+  </si>
+  <si>
+    <t>jde to, je to v poho</t>
+  </si>
+  <si>
+    <t>tohle je dobry, krome toho co znamena Podprostor</t>
   </si>
 </sst>
 </file>
@@ -901,8 +976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E55586A-675C-45F4-B755-48CD8B419B21}">
   <dimension ref="A1:T50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -913,9 +988,8 @@
     <col min="4" max="4" width="39.77734375" customWidth="1"/>
     <col min="5" max="5" width="51.88671875" customWidth="1"/>
     <col min="6" max="6" width="11.5546875" customWidth="1"/>
-    <col min="7" max="7" width="39.5546875" customWidth="1"/>
-    <col min="8" max="8" width="9.44140625" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" customWidth="1"/>
+    <col min="7" max="7" width="175.88671875" customWidth="1"/>
+    <col min="8" max="9" width="9.44140625" customWidth="1"/>
     <col min="10" max="10" width="9.33203125" customWidth="1"/>
     <col min="11" max="11" width="11.5546875" customWidth="1"/>
     <col min="13" max="13" width="49.88671875" customWidth="1"/>
@@ -931,7 +1005,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D1" s="16"/>
       <c r="E1" s="8" t="s">
@@ -941,7 +1015,7 @@
         <v>0</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H1" s="3"/>
       <c r="I1" s="6"/>
@@ -972,10 +1046,10 @@
         <v>43</v>
       </c>
       <c r="F2" s="12">
-        <v>5</v>
+        <v>3.4</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="4"/>
@@ -1006,10 +1080,10 @@
         <v>44</v>
       </c>
       <c r="F3" s="12">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>2</v>
+        <v>73</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="4"/>
@@ -1040,10 +1114,10 @@
         <v>45</v>
       </c>
       <c r="F4" s="12">
-        <v>5</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>2</v>
+        <v>99</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="4"/>
@@ -1064,20 +1138,20 @@
         <v>6</v>
       </c>
       <c r="B5" s="17">
-        <v>5</v>
+        <v>1.2</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="D5" s="16"/>
       <c r="E5" s="13" t="s">
         <v>46</v>
       </c>
       <c r="F5" s="12">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>2</v>
+        <v>98</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="4"/>
@@ -1098,20 +1172,20 @@
         <v>12</v>
       </c>
       <c r="B6" s="17">
-        <v>4</v>
+        <v>3.4</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D6" s="16"/>
       <c r="E6" s="13" t="s">
         <v>47</v>
       </c>
       <c r="F6" s="12">
-        <v>5</v>
+        <v>1.2</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="4"/>
@@ -1132,20 +1206,20 @@
         <v>7</v>
       </c>
       <c r="B7" s="17">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>2</v>
+        <v>88</v>
       </c>
       <c r="D7" s="16"/>
       <c r="E7" s="13" t="s">
         <v>48</v>
       </c>
       <c r="F7" s="12">
-        <v>5</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="4"/>
@@ -1166,20 +1240,20 @@
         <v>8</v>
       </c>
       <c r="B8" s="17">
-        <v>5</v>
+        <v>3.4</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>2</v>
+        <v>89</v>
       </c>
       <c r="D8" s="16"/>
       <c r="E8" s="13" t="s">
         <v>49</v>
       </c>
       <c r="F8" s="12">
-        <v>5</v>
+        <v>1.2</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="4"/>
@@ -1210,10 +1284,10 @@
         <v>50</v>
       </c>
       <c r="F9" s="12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>2</v>
+        <v>75</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="4"/>
@@ -1244,10 +1318,10 @@
         <v>51</v>
       </c>
       <c r="F10" s="12">
-        <v>5</v>
+        <v>3.4</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>2</v>
+        <v>76</v>
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="4"/>
@@ -1278,10 +1352,10 @@
         <v>52</v>
       </c>
       <c r="F11" s="12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>2</v>
+        <v>77</v>
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="4"/>
@@ -1312,10 +1386,10 @@
         <v>53</v>
       </c>
       <c r="F12" s="12">
-        <v>5</v>
+        <v>3.4</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>2</v>
+        <v>78</v>
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="4"/>
@@ -1346,10 +1420,10 @@
         <v>54</v>
       </c>
       <c r="F13" s="12">
-        <v>5</v>
+        <v>3.4</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>2</v>
+        <v>79</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="4"/>
@@ -1380,10 +1454,10 @@
         <v>55</v>
       </c>
       <c r="F14" s="12">
-        <v>5</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>2</v>
+        <v>80</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="4"/>
@@ -1414,10 +1488,10 @@
         <v>56</v>
       </c>
       <c r="F15" s="12">
-        <v>5</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>2</v>
+        <v>81</v>
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="4"/>
@@ -1448,10 +1522,10 @@
         <v>57</v>
       </c>
       <c r="F16" s="12">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>2</v>
+        <v>82</v>
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="4"/>
@@ -1482,10 +1556,10 @@
         <v>58</v>
       </c>
       <c r="F17" s="12">
-        <v>5</v>
+        <v>3.4</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>2</v>
+        <v>83</v>
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="4"/>
@@ -1516,10 +1590,10 @@
         <v>59</v>
       </c>
       <c r="F18" s="12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>2</v>
+        <v>84</v>
       </c>
       <c r="H18" s="3"/>
       <c r="I18" s="4"/>
@@ -1550,10 +1624,10 @@
         <v>60</v>
       </c>
       <c r="F19" s="12">
-        <v>5</v>
+        <v>1.2</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>2</v>
+        <v>85</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
@@ -1584,10 +1658,10 @@
         <v>61</v>
       </c>
       <c r="F20" s="12">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>2</v>
+        <v>86</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -1618,10 +1692,10 @@
         <v>62</v>
       </c>
       <c r="F21" s="12">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>2</v>
+        <v>87</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -1652,10 +1726,10 @@
         <v>63</v>
       </c>
       <c r="F22" s="12">
-        <v>5</v>
+        <v>3.4</v>
       </c>
       <c r="G22" s="15" t="s">
-        <v>2</v>
+        <v>90</v>
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
@@ -1686,10 +1760,10 @@
         <v>64</v>
       </c>
       <c r="F23" s="12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G23" s="15" t="s">
-        <v>2</v>
+        <v>91</v>
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
@@ -1720,10 +1794,10 @@
         <v>65</v>
       </c>
       <c r="F24" s="12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>2</v>
+        <v>92</v>
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
@@ -1754,10 +1828,10 @@
         <v>66</v>
       </c>
       <c r="F25" s="12">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G25" s="15" t="s">
-        <v>2</v>
+        <v>93</v>
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
@@ -1788,10 +1862,10 @@
         <v>67</v>
       </c>
       <c r="F26" s="12">
-        <v>5</v>
+        <v>1.2</v>
       </c>
       <c r="G26" s="15" t="s">
-        <v>2</v>
+        <v>94</v>
       </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>

</xml_diff>

<commit_message>
Deployed dbb0a6d with MkDocs version: 1.6.1
</commit_message>
<xml_diff>
--- a/linearni_algerbra_diskretni_mat/Algebra_TABULKA.xlsx
+++ b/linearni_algerbra_diskretni_mat/Algebra_TABULKA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dejvi\Plocha\TUL\docs\linearni_algerbra_diskretni_mat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17000595-319E-46A8-947D-5B1F406AF210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADA32CA-5F5E-4369-A5F2-350B87518460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="13023" tabRatio="567" xr2:uid="{0AD5C3A5-6B82-437D-9C85-E9151057B14B}"/>
   </bookViews>
@@ -263,24 +263,12 @@
     <t>praktické téma, docela jde</t>
   </si>
   <si>
-    <t>podobné 1 ale je tam par věci  co nejsou zastak jednoduchy</t>
-  </si>
-  <si>
     <t>proste tohle nam říká zda mame vůbec reseni</t>
   </si>
   <si>
-    <t>je to nic moc ale není to až tak dlouhy</t>
-  </si>
-  <si>
     <t>docela jde, něco vim prakticky</t>
   </si>
   <si>
-    <t>podobné 11 ale mozna trosku lehci</t>
-  </si>
-  <si>
-    <t>jednoduší než téma 7</t>
-  </si>
-  <si>
     <t>není to ažtak obtížné</t>
   </si>
   <si>
@@ -336,6 +324,18 @@
   </si>
   <si>
     <t>tohle je dobry, krome toho co znamena Podprostor</t>
+  </si>
+  <si>
+    <t>podobne 1, ale kratsi</t>
+  </si>
+  <si>
+    <t>da se v tom chybovat ale jde docela</t>
+  </si>
+  <si>
+    <t>podobné 11</t>
+  </si>
+  <si>
+    <t>hodne v pohodě</t>
   </si>
 </sst>
 </file>
@@ -976,8 +976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E55586A-675C-45F4-B755-48CD8B419B21}">
   <dimension ref="A1:T50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="D5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -1049,7 +1049,7 @@
         <v>3.4</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="4"/>
@@ -1117,7 +1117,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="4"/>
@@ -1141,7 +1141,7 @@
         <v>1.2</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D5" s="16"/>
       <c r="E5" s="13" t="s">
@@ -1151,7 +1151,7 @@
         <v>2</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="4"/>
@@ -1185,7 +1185,7 @@
         <v>1.2</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="4"/>
@@ -1209,7 +1209,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D7" s="16"/>
       <c r="E7" s="13" t="s">
@@ -1219,7 +1219,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="4"/>
@@ -1243,7 +1243,7 @@
         <v>3.4</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D8" s="16"/>
       <c r="E8" s="13" t="s">
@@ -1284,10 +1284,10 @@
         <v>50</v>
       </c>
       <c r="F9" s="12">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="4"/>
@@ -1318,10 +1318,10 @@
         <v>51</v>
       </c>
       <c r="F10" s="12">
-        <v>3.4</v>
+        <v>1.2</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="4"/>
@@ -1352,10 +1352,10 @@
         <v>52</v>
       </c>
       <c r="F11" s="12">
-        <v>4</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="4"/>
@@ -1386,10 +1386,10 @@
         <v>53</v>
       </c>
       <c r="F12" s="12">
-        <v>3.4</v>
+        <v>1.2</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="4"/>
@@ -1420,10 +1420,10 @@
         <v>54</v>
       </c>
       <c r="F13" s="12">
-        <v>3.4</v>
+        <v>2</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="4"/>
@@ -1454,10 +1454,10 @@
         <v>55</v>
       </c>
       <c r="F14" s="12">
-        <v>2.2999999999999998</v>
+        <v>1.2</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>80</v>
+        <v>99</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="4"/>
@@ -1488,10 +1488,10 @@
         <v>56</v>
       </c>
       <c r="F15" s="12">
-        <v>2.2999999999999998</v>
+        <v>1.2</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="4"/>
@@ -1525,7 +1525,7 @@
         <v>3</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="4"/>
@@ -1559,7 +1559,7 @@
         <v>3.4</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="4"/>
@@ -1593,7 +1593,7 @@
         <v>4</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H18" s="3"/>
       <c r="I18" s="4"/>
@@ -1627,7 +1627,7 @@
         <v>1.2</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
@@ -1661,7 +1661,7 @@
         <v>2</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -1695,7 +1695,7 @@
         <v>2</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -1729,7 +1729,7 @@
         <v>3.4</v>
       </c>
       <c r="G22" s="15" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
@@ -1763,7 +1763,7 @@
         <v>4</v>
       </c>
       <c r="G23" s="15" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
@@ -1797,7 +1797,7 @@
         <v>4</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
@@ -1831,7 +1831,7 @@
         <v>2</v>
       </c>
       <c r="G25" s="15" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
@@ -1865,7 +1865,7 @@
         <v>1.2</v>
       </c>
       <c r="G26" s="15" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>

</xml_diff>

<commit_message>
Deployed a50199a with MkDocs version: 1.6.1
</commit_message>
<xml_diff>
--- a/linearni_algerbra_diskretni_mat/Algebra_TABULKA.xlsx
+++ b/linearni_algerbra_diskretni_mat/Algebra_TABULKA.xlsx
@@ -2,34 +2,23 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dejvi\Plocha\TUL\docs\linearni_algerbra_diskretni_mat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dejvi\Desktop\TUL\docs\linearni_algerbra_diskretni_mat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADA32CA-5F5E-4369-A5F2-350B87518460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D0B70B-E60D-4BC5-A9AE-D441F23588AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="13023" tabRatio="567" xr2:uid="{0AD5C3A5-6B82-437D-9C85-E9151057B14B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="567" xr2:uid="{0AD5C3A5-6B82-437D-9C85-E9151057B14B}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -296,12 +285,6 @@
     <t>nedelat chyby v GEM</t>
   </si>
   <si>
-    <t>vzorců tam je extrémně moc</t>
-  </si>
-  <si>
-    <t>extrém</t>
-  </si>
-  <si>
     <t>prakticky trochu podobné tématu 11 a navazuje to na tema 22</t>
   </si>
   <si>
@@ -336,6 +319,12 @@
   </si>
   <si>
     <t>hodne v pohodě</t>
+  </si>
+  <si>
+    <t>vzorců tam je hodne ale dá se to</t>
+  </si>
+  <si>
+    <t>extrém, ale dá se</t>
   </si>
 </sst>
 </file>
@@ -976,28 +965,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E55586A-675C-45F4-B755-48CD8B419B21}">
   <dimension ref="A1:T50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="D13" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="58.5546875" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" customWidth="1"/>
-    <col min="3" max="3" width="39.33203125" customWidth="1"/>
-    <col min="4" max="4" width="39.77734375" customWidth="1"/>
-    <col min="5" max="5" width="51.88671875" customWidth="1"/>
-    <col min="6" max="6" width="11.5546875" customWidth="1"/>
-    <col min="7" max="7" width="175.88671875" customWidth="1"/>
-    <col min="8" max="9" width="9.44140625" customWidth="1"/>
-    <col min="10" max="10" width="9.33203125" customWidth="1"/>
-    <col min="11" max="11" width="11.5546875" customWidth="1"/>
-    <col min="13" max="13" width="49.88671875" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="58.54296875" customWidth="1"/>
+    <col min="2" max="2" width="11.6328125" customWidth="1"/>
+    <col min="3" max="3" width="39.36328125" customWidth="1"/>
+    <col min="4" max="4" width="39.81640625" customWidth="1"/>
+    <col min="5" max="5" width="51.90625" customWidth="1"/>
+    <col min="6" max="6" width="11.54296875" customWidth="1"/>
+    <col min="7" max="7" width="141.26953125" customWidth="1"/>
+    <col min="8" max="9" width="9.453125" customWidth="1"/>
+    <col min="10" max="10" width="9.36328125" customWidth="1"/>
+    <col min="11" max="11" width="11.54296875" customWidth="1"/>
+    <col min="13" max="13" width="49.90625" customWidth="1"/>
+    <col min="14" max="14" width="10.6328125" customWidth="1"/>
     <col min="16" max="16" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
@@ -1031,7 +1020,7 @@
       <c r="S1" s="2"/>
       <c r="T1" s="2"/>
     </row>
-    <row r="2" spans="1:20" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="11" t="s">
         <v>4</v>
       </c>
@@ -1046,10 +1035,10 @@
         <v>43</v>
       </c>
       <c r="F2" s="12">
-        <v>3.4</v>
+        <v>3</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="4"/>
@@ -1065,7 +1054,7 @@
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
     </row>
-    <row r="3" spans="1:20" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="13" t="s">
         <v>3</v>
       </c>
@@ -1099,7 +1088,7 @@
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
     </row>
-    <row r="4" spans="1:20" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="13" t="s">
         <v>5</v>
       </c>
@@ -1117,7 +1106,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="4"/>
@@ -1133,7 +1122,7 @@
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
     </row>
-    <row r="5" spans="1:20" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="13" t="s">
         <v>6</v>
       </c>
@@ -1141,7 +1130,7 @@
         <v>1.2</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D5" s="16"/>
       <c r="E5" s="13" t="s">
@@ -1151,7 +1140,7 @@
         <v>2</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="4"/>
@@ -1167,7 +1156,7 @@
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
     </row>
-    <row r="6" spans="1:20" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" s="13" t="s">
         <v>12</v>
       </c>
@@ -1185,7 +1174,7 @@
         <v>1.2</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="4"/>
@@ -1201,7 +1190,7 @@
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="1:20" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7" s="13" t="s">
         <v>7</v>
       </c>
@@ -1219,7 +1208,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="4"/>
@@ -1235,7 +1224,7 @@
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
     </row>
-    <row r="8" spans="1:20" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="13" t="s">
         <v>8</v>
       </c>
@@ -1269,7 +1258,7 @@
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
     </row>
-    <row r="9" spans="1:20" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="13" t="s">
         <v>9</v>
       </c>
@@ -1287,7 +1276,7 @@
         <v>2</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="4"/>
@@ -1303,7 +1292,7 @@
       <c r="S9" s="2"/>
       <c r="T9" s="2"/>
     </row>
-    <row r="10" spans="1:20" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A10" s="13" t="s">
         <v>10</v>
       </c>
@@ -1337,7 +1326,7 @@
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
     </row>
-    <row r="11" spans="1:20" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A11" s="13" t="s">
         <v>11</v>
       </c>
@@ -1355,7 +1344,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="4"/>
@@ -1371,7 +1360,7 @@
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
     </row>
-    <row r="12" spans="1:20" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A12" s="13" t="s">
         <v>13</v>
       </c>
@@ -1405,7 +1394,7 @@
       <c r="S12" s="2"/>
       <c r="T12" s="2"/>
     </row>
-    <row r="13" spans="1:20" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13" s="13" t="s">
         <v>14</v>
       </c>
@@ -1423,7 +1412,7 @@
         <v>2</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="4"/>
@@ -1439,7 +1428,7 @@
       <c r="S13" s="2"/>
       <c r="T13" s="2"/>
     </row>
-    <row r="14" spans="1:20" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" s="13" t="s">
         <v>15</v>
       </c>
@@ -1457,7 +1446,7 @@
         <v>1.2</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="4"/>
@@ -1473,7 +1462,7 @@
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
     </row>
-    <row r="15" spans="1:20" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A15" s="13" t="s">
         <v>16</v>
       </c>
@@ -1507,7 +1496,7 @@
       <c r="S15" s="2"/>
       <c r="T15" s="2"/>
     </row>
-    <row r="16" spans="1:20" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A16" s="13" t="s">
         <v>17</v>
       </c>
@@ -1522,7 +1511,7 @@
         <v>57</v>
       </c>
       <c r="F16" s="12">
-        <v>3</v>
+        <v>1.2</v>
       </c>
       <c r="G16" s="15" t="s">
         <v>78</v>
@@ -1541,7 +1530,7 @@
       <c r="S16" s="2"/>
       <c r="T16" s="2"/>
     </row>
-    <row r="17" spans="1:20" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A17" s="13" t="s">
         <v>18</v>
       </c>
@@ -1556,7 +1545,7 @@
         <v>58</v>
       </c>
       <c r="F17" s="12">
-        <v>3.4</v>
+        <v>2</v>
       </c>
       <c r="G17" s="15" t="s">
         <v>79</v>
@@ -1575,7 +1564,7 @@
       <c r="S17" s="2"/>
       <c r="T17" s="2"/>
     </row>
-    <row r="18" spans="1:20" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A18" s="13" t="s">
         <v>19</v>
       </c>
@@ -1590,7 +1579,7 @@
         <v>59</v>
       </c>
       <c r="F18" s="12">
-        <v>4</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="G18" s="15" t="s">
         <v>80</v>
@@ -1609,7 +1598,7 @@
       <c r="S18" s="2"/>
       <c r="T18" s="2"/>
     </row>
-    <row r="19" spans="1:20" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A19" s="13" t="s">
         <v>20</v>
       </c>
@@ -1643,7 +1632,7 @@
       <c r="S19" s="2"/>
       <c r="T19" s="2"/>
     </row>
-    <row r="20" spans="1:20" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A20" s="13" t="s">
         <v>21</v>
       </c>
@@ -1658,7 +1647,7 @@
         <v>61</v>
       </c>
       <c r="F20" s="12">
-        <v>2</v>
+        <v>1.2</v>
       </c>
       <c r="G20" s="15" t="s">
         <v>82</v>
@@ -1677,7 +1666,7 @@
       <c r="S20" s="2"/>
       <c r="T20" s="2"/>
     </row>
-    <row r="21" spans="1:20" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A21" s="14" t="s">
         <v>22</v>
       </c>
@@ -1692,7 +1681,7 @@
         <v>62</v>
       </c>
       <c r="F21" s="12">
-        <v>2</v>
+        <v>1.2</v>
       </c>
       <c r="G21" s="15" t="s">
         <v>83</v>
@@ -1711,7 +1700,7 @@
       <c r="S21" s="2"/>
       <c r="T21" s="2"/>
     </row>
-    <row r="22" spans="1:20" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A22" s="14" t="s">
         <v>24</v>
       </c>
@@ -1726,10 +1715,10 @@
         <v>63</v>
       </c>
       <c r="F22" s="12">
-        <v>3.4</v>
+        <v>2</v>
       </c>
       <c r="G22" s="15" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
@@ -1745,7 +1734,7 @@
       <c r="S22" s="2"/>
       <c r="T22" s="2"/>
     </row>
-    <row r="23" spans="1:20" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A23" s="14" t="s">
         <v>25</v>
       </c>
@@ -1760,10 +1749,10 @@
         <v>64</v>
       </c>
       <c r="F23" s="12">
-        <v>4</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="G23" s="15" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
@@ -1779,7 +1768,7 @@
       <c r="S23" s="2"/>
       <c r="T23" s="2"/>
     </row>
-    <row r="24" spans="1:20" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A24" s="14" t="s">
         <v>26</v>
       </c>
@@ -1794,10 +1783,10 @@
         <v>65</v>
       </c>
       <c r="F24" s="12">
-        <v>4</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
@@ -1813,7 +1802,7 @@
       <c r="S24" s="2"/>
       <c r="T24" s="2"/>
     </row>
-    <row r="25" spans="1:20" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A25" s="14" t="s">
         <v>27</v>
       </c>
@@ -1828,10 +1817,10 @@
         <v>66</v>
       </c>
       <c r="F25" s="12">
-        <v>2</v>
+        <v>1.2</v>
       </c>
       <c r="G25" s="15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
@@ -1847,7 +1836,7 @@
       <c r="S25" s="2"/>
       <c r="T25" s="2"/>
     </row>
-    <row r="26" spans="1:20" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A26" s="14" t="s">
         <v>29</v>
       </c>
@@ -1865,7 +1854,7 @@
         <v>1.2</v>
       </c>
       <c r="G26" s="15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
@@ -1881,7 +1870,7 @@
       <c r="S26" s="2"/>
       <c r="T26" s="2"/>
     </row>
-    <row r="27" spans="1:20" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A27" s="14" t="s">
         <v>28</v>
       </c>
@@ -1909,7 +1898,7 @@
       <c r="S27" s="2"/>
       <c r="T27" s="2"/>
     </row>
-    <row r="28" spans="1:20" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A28" s="14" t="s">
         <v>30</v>
       </c>
@@ -1937,7 +1926,7 @@
       <c r="S28" s="2"/>
       <c r="T28" s="2"/>
     </row>
-    <row r="29" spans="1:20" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A29" s="14" t="s">
         <v>31</v>
       </c>
@@ -1953,7 +1942,7 @@
       <c r="G29" s="16"/>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="1:20" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A30" s="14" t="s">
         <v>32</v>
       </c>
@@ -1969,7 +1958,7 @@
       <c r="G30" s="16"/>
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="1:20" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A31" s="14" t="s">
         <v>33</v>
       </c>
@@ -1985,7 +1974,7 @@
       <c r="G31" s="16"/>
       <c r="H31" s="1"/>
     </row>
-    <row r="32" spans="1:20" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A32" s="14" t="s">
         <v>34</v>
       </c>
@@ -2001,7 +1990,7 @@
       <c r="G32" s="16"/>
       <c r="H32" s="1"/>
     </row>
-    <row r="33" spans="1:8" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A33" s="14" t="s">
         <v>35</v>
       </c>
@@ -2017,7 +2006,7 @@
       <c r="G33" s="16"/>
       <c r="H33" s="1"/>
     </row>
-    <row r="34" spans="1:8" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A34" s="14" t="s">
         <v>37</v>
       </c>
@@ -2033,7 +2022,7 @@
       <c r="G34" s="16"/>
       <c r="H34" s="1"/>
     </row>
-    <row r="35" spans="1:8" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A35" s="14" t="s">
         <v>38</v>
       </c>
@@ -2049,7 +2038,7 @@
       <c r="G35" s="16"/>
       <c r="H35" s="1"/>
     </row>
-    <row r="36" spans="1:8" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A36" s="14" t="s">
         <v>36</v>
       </c>
@@ -2064,7 +2053,7 @@
       <c r="F36" s="16"/>
       <c r="G36" s="16"/>
     </row>
-    <row r="37" spans="1:8" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A37" s="14" t="s">
         <v>39</v>
       </c>
@@ -2079,7 +2068,7 @@
       <c r="F37" s="16"/>
       <c r="G37" s="16"/>
     </row>
-    <row r="38" spans="1:8" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A38" s="14" t="s">
         <v>40</v>
       </c>
@@ -2094,7 +2083,7 @@
       <c r="F38" s="16"/>
       <c r="G38" s="16"/>
     </row>
-    <row r="39" spans="1:8" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A39" s="14" t="s">
         <v>41</v>
       </c>
@@ -2109,7 +2098,7 @@
       <c r="F39" s="16"/>
       <c r="G39" s="16"/>
     </row>
-    <row r="40" spans="1:8" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A40" s="14" t="s">
         <v>42</v>
       </c>
@@ -2124,16 +2113,16 @@
       <c r="F40" s="16"/>
       <c r="G40" s="16"/>
     </row>
-    <row r="41" spans="1:8" ht="30.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="1:8" ht="30.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="1:8" ht="30.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="1:8" ht="30.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="1:8" ht="30.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="46" spans="1:8" ht="30.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="47" spans="1:8" ht="30.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="48" spans="1:8" ht="30.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="49" ht="30.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="50" ht="30.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="42" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="43" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="44" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="45" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="46" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="47" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="48" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="49" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="50" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="B2:B40">

</xml_diff>